<commit_message>
just test in another computer
</commit_message>
<xml_diff>
--- a/data_output/shift_kosong.xlsx
+++ b/data_output/shift_kosong.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="kosong" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="kosong" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>6067</v>
+        <v>6065</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>6068</v>
+        <v>6066</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>6069</v>
+        <v>6067</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>7798</v>
+        <v>7796</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>7799</v>
+        <v>7797</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>7800</v>
+        <v>7798</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2248,7 +2248,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>9172</v>
+        <v>9170</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>9173</v>
+        <v>9171</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>

</xml_diff>